<commit_message>
Genarate some additional packages
</commit_message>
<xml_diff>
--- a/course/day_5/example.xlsx
+++ b/course/day_5/example.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/GitLab/pyt/course/day_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00AA969-F793-0F4A-82BD-F4AC67CE2DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2236ABC8-7D8A-F14C-AE42-EB84AD99FB84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="820" windowWidth="28240" windowHeight="16920" xr2:uid="{1B6E11E4-0C14-4041-9D45-C8B511705C1A}"/>
+    <workbookView xWindow="8100" yWindow="800" windowWidth="28240" windowHeight="16920" activeTab="1" xr2:uid="{1B6E11E4-0C14-4041-9D45-C8B511705C1A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Früchte" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA69524-D36D-1747-A909-0D9FBC41C089}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>4711</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -536,10 +536,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B860ABD-889E-4947-94CA-C77529B66077}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D44761-2FFD-6444-9E56-BD99E4B3D5D6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>

</xml_diff>